<commit_message>
Changed snow height netcdf, so if there are no data for an entire month - use last valid measurement at report in comments.
</commit_message>
<xml_diff>
--- a/metadata/snd_metadata.xlsx
+++ b/metadata/snd_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67572B79-8A41-3A4E-A16B-8E6AA43DFE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2293AF56-19CA-6D4B-8225-C9269F2FBBB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="-3140" windowWidth="28420" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31500" yWindow="-3140" windowWidth="28420" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -704,7 +704,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updates for July 2021 raise
</commit_message>
<xml_diff>
--- a/metadata/snd_metadata.xlsx
+++ b/metadata/snd_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2293AF56-19CA-6D4B-8225-C9269F2FBBB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262A9132-894C-6546-AACA-44B1270B8EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="-3140" windowWidth="28420" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31500" yWindow="460" windowWidth="28420" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>Data collection start: 2019-06-01T00:00:00</t>
-  </si>
-  <si>
-    <t>Platform height is the top of the Met tower, sensor height is plaform height minus 12.3 m.</t>
   </si>
   <si>
     <t>CF-1.6</t>
@@ -259,6 +256,9 @@
   </si>
   <si>
     <t>timeSeries</t>
+  </si>
+  <si>
+    <t>Platform height is the top of the Met tower, sensor height is plaform height minus 10.83 m.</t>
   </si>
 </sst>
 </file>
@@ -370,14 +370,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -403,7 +403,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -704,7 +704,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -727,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -815,7 +815,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -847,7 +847,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -933,7 +933,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -965,7 +965,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -973,7 +973,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -993,7 +993,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1036,7 +1036,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>